<commit_message>
updated excel that'll be removed when finished
</commit_message>
<xml_diff>
--- a/PythonStuff/commandsExcelExample.xlsx
+++ b/PythonStuff/commandsExcelExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andyclarkson/Desktop/BYU-I/Spring-22/CSE-212/Final/PythonStuff/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA7110A2-D551-AB42-9B68-63478953B210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BEE283-6912-B646-9C9C-2E2C81CE127D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="5760" windowWidth="33320" windowHeight="16640" xr2:uid="{EDF841D6-2216-AF4F-91D0-5805F50CAB89}"/>
+    <workbookView xWindow="1080" yWindow="5760" windowWidth="34760" windowHeight="16640" xr2:uid="{EDF841D6-2216-AF4F-91D0-5805F50CAB89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="23">
   <si>
     <t>Command Operation</t>
   </si>
@@ -364,19 +364,10 @@
   </cellStyleXfs>
   <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -385,19 +376,55 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -406,49 +433,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -457,11 +445,20 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -469,11 +466,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -789,288 +789,477 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D3AA607-3827-0C4A-96B7-E3DD9D91A22D}">
-  <dimension ref="D6:K23"/>
+  <dimension ref="D6:AA23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16:I17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D6" s="1" t="s">
+    <row r="6" spans="4:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="37"/>
+      <c r="T6" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" s="37"/>
+      <c r="V6" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
+      <c r="W6" s="37"/>
+      <c r="X6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1" t="s">
+      <c r="Y6" s="37"/>
+      <c r="Z6" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D8" s="2" t="s">
+      <c r="AA6" s="37"/>
+    </row>
+    <row r="7" spans="4:27" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="37"/>
+      <c r="W7" s="37"/>
+      <c r="X7" s="37"/>
+      <c r="Y7" s="37"/>
+      <c r="Z7" s="37"/>
+      <c r="AA7" s="37"/>
+    </row>
+    <row r="8" spans="4:27" x14ac:dyDescent="0.2">
+      <c r="D8" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="34" t="s">
+      <c r="E8" s="31"/>
+      <c r="F8" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="34"/>
-      <c r="J8" s="5" t="s">
+      <c r="G8" s="33"/>
+      <c r="H8" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="5"/>
-    </row>
-    <row r="9" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-    </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D10" s="23" t="s">
+      <c r="I8" s="35"/>
+      <c r="T8" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="U8" s="31"/>
+      <c r="V8" s="32"/>
+      <c r="W8" s="30"/>
+      <c r="X8" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y8" s="33"/>
+      <c r="Z8" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA8" s="35"/>
+    </row>
+    <row r="9" spans="4:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="22"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="34"/>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="36"/>
+      <c r="AA9" s="36"/>
+    </row>
+    <row r="10" spans="4:27" x14ac:dyDescent="0.2">
+      <c r="D10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="36" t="s">
+      <c r="E10" s="12"/>
+      <c r="F10" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="36"/>
-      <c r="J10" s="16" t="s">
+      <c r="G10" s="17"/>
+      <c r="H10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="16"/>
-    </row>
-    <row r="11" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-    </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D12" s="19" t="s">
+      <c r="I10" s="9"/>
+      <c r="T10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="U10" s="12"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA10" s="9"/>
+    </row>
+    <row r="11" spans="4:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="19"/>
+    </row>
+    <row r="12" spans="4:27" x14ac:dyDescent="0.2">
+      <c r="D12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="30" t="s">
+      <c r="E12" s="21"/>
+      <c r="F12" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="30"/>
-      <c r="J12" s="22" t="s">
+      <c r="G12" s="26"/>
+      <c r="H12" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="22"/>
-    </row>
-    <row r="13" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D14" s="10" t="s">
+      <c r="I12" s="28"/>
+      <c r="T12" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="U12" s="21"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y12" s="26"/>
+      <c r="Z12" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA12" s="28"/>
+    </row>
+    <row r="13" spans="4:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="22"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="T13" s="22"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="25"/>
+      <c r="W13" s="22"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="29"/>
+      <c r="AA13" s="29"/>
+    </row>
+    <row r="14" spans="4:27" x14ac:dyDescent="0.2">
+      <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="32" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="32"/>
-      <c r="J14" s="16" t="s">
+      <c r="G14" s="7"/>
+      <c r="H14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="16"/>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
+      <c r="I14" s="9"/>
+      <c r="T14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U14" s="2"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA14" s="9"/>
+    </row>
+    <row r="15" spans="4:27" x14ac:dyDescent="0.2">
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D16" s="2" t="s">
+      <c r="G15" s="8"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="10"/>
+    </row>
+    <row r="16" spans="4:27" x14ac:dyDescent="0.2">
+      <c r="D16" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="34" t="s">
+      <c r="E16" s="31"/>
+      <c r="F16" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="34"/>
-      <c r="J16" s="5" t="s">
+      <c r="G16" s="33"/>
+      <c r="H16" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D18" s="23" t="s">
+      <c r="I16" s="35"/>
+      <c r="T16" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="U16" s="31"/>
+      <c r="V16" s="32"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y16" s="33"/>
+      <c r="Z16" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA16" s="35"/>
+    </row>
+    <row r="17" spans="4:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="22"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="34"/>
+      <c r="Y17" s="34"/>
+      <c r="Z17" s="36"/>
+      <c r="AA17" s="36"/>
+    </row>
+    <row r="18" spans="4:27" x14ac:dyDescent="0.2">
+      <c r="D18" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="36" t="s">
+      <c r="E18" s="12"/>
+      <c r="F18" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I18" s="36"/>
-      <c r="J18" s="16" t="s">
+      <c r="G18" s="17"/>
+      <c r="H18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K18" s="16"/>
-    </row>
-    <row r="19" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="26"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D20" s="19" t="s">
+      <c r="I18" s="9"/>
+      <c r="T18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="U18" s="12"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA18" s="9"/>
+    </row>
+    <row r="19" spans="4:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="13"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="14"/>
+      <c r="V19" s="16"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="18"/>
+      <c r="Y19" s="18"/>
+      <c r="Z19" s="19"/>
+      <c r="AA19" s="19"/>
+    </row>
+    <row r="20" spans="4:27" x14ac:dyDescent="0.2">
+      <c r="D20" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="30" t="s">
+      <c r="E20" s="21"/>
+      <c r="F20" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="30"/>
-      <c r="J20" s="22" t="s">
+      <c r="G20" s="26"/>
+      <c r="H20" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="K20" s="22"/>
-    </row>
-    <row r="21" spans="4:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="13"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D22" s="10" t="s">
+      <c r="I20" s="28"/>
+      <c r="T20" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="U20" s="21"/>
+      <c r="V20" s="24"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y20" s="26"/>
+      <c r="Z20" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA20" s="28"/>
+    </row>
+    <row r="21" spans="4:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="22"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="T21" s="22"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="25"/>
+      <c r="W21" s="22"/>
+      <c r="X21" s="27"/>
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="29"/>
+      <c r="AA21" s="29"/>
+    </row>
+    <row r="22" spans="4:27" x14ac:dyDescent="0.2">
+      <c r="D22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="32" t="s">
+      <c r="E22" s="2"/>
+      <c r="F22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="32"/>
-      <c r="J22" s="16" t="s">
+      <c r="G22" s="7"/>
+      <c r="H22" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K22" s="16"/>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
+      <c r="I22" s="9"/>
+      <c r="T22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U22" s="2"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y22" s="7"/>
+      <c r="Z22" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA22" s="9"/>
+    </row>
+    <row r="23" spans="4:27" x14ac:dyDescent="0.2">
+      <c r="D23" s="3"/>
+      <c r="E23" s="4"/>
       <c r="F23" s="8"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="63">
+    <mergeCell ref="T22:U23"/>
+    <mergeCell ref="V22:W23"/>
+    <mergeCell ref="X22:Y23"/>
+    <mergeCell ref="Z22:AA23"/>
+    <mergeCell ref="T18:U19"/>
+    <mergeCell ref="V18:W19"/>
+    <mergeCell ref="X18:Y19"/>
+    <mergeCell ref="Z18:AA19"/>
+    <mergeCell ref="T20:U21"/>
+    <mergeCell ref="V20:W21"/>
+    <mergeCell ref="X20:Y21"/>
+    <mergeCell ref="Z20:AA21"/>
+    <mergeCell ref="T14:U15"/>
+    <mergeCell ref="V14:W15"/>
+    <mergeCell ref="X14:Y15"/>
+    <mergeCell ref="Z14:AA15"/>
+    <mergeCell ref="T16:U17"/>
+    <mergeCell ref="V16:W17"/>
+    <mergeCell ref="X16:Y17"/>
+    <mergeCell ref="Z16:AA17"/>
+    <mergeCell ref="T10:U11"/>
+    <mergeCell ref="V10:W11"/>
+    <mergeCell ref="X10:Y11"/>
+    <mergeCell ref="Z10:AA11"/>
+    <mergeCell ref="T12:U13"/>
+    <mergeCell ref="V12:W13"/>
+    <mergeCell ref="X12:Y13"/>
+    <mergeCell ref="Z12:AA13"/>
+    <mergeCell ref="T6:U7"/>
+    <mergeCell ref="V6:W7"/>
+    <mergeCell ref="X6:Y7"/>
+    <mergeCell ref="Z6:AA7"/>
+    <mergeCell ref="T8:U9"/>
+    <mergeCell ref="V8:W9"/>
+    <mergeCell ref="X8:Y9"/>
+    <mergeCell ref="Z8:AA9"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="F6:G7"/>
+    <mergeCell ref="H6:I7"/>
+    <mergeCell ref="H8:I9"/>
+    <mergeCell ref="F8:G9"/>
+    <mergeCell ref="D8:E9"/>
+    <mergeCell ref="D10:E11"/>
+    <mergeCell ref="F10:G11"/>
+    <mergeCell ref="H10:I11"/>
+    <mergeCell ref="D12:E13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="H12:I13"/>
+    <mergeCell ref="D14:E15"/>
+    <mergeCell ref="F14:G15"/>
+    <mergeCell ref="H14:I15"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F16:G17"/>
+    <mergeCell ref="H16:I17"/>
     <mergeCell ref="D22:E23"/>
     <mergeCell ref="F22:G23"/>
     <mergeCell ref="H22:I23"/>
-    <mergeCell ref="J22:K23"/>
     <mergeCell ref="D18:E19"/>
     <mergeCell ref="F18:G19"/>
     <mergeCell ref="H18:I19"/>
-    <mergeCell ref="J18:K19"/>
     <mergeCell ref="D20:E21"/>
     <mergeCell ref="F20:G21"/>
     <mergeCell ref="H20:I21"/>
-    <mergeCell ref="J20:K21"/>
-    <mergeCell ref="D14:E15"/>
-    <mergeCell ref="F14:G15"/>
-    <mergeCell ref="H14:I15"/>
-    <mergeCell ref="J14:K15"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="F16:G17"/>
-    <mergeCell ref="H16:I17"/>
-    <mergeCell ref="J16:K17"/>
-    <mergeCell ref="D10:E11"/>
-    <mergeCell ref="F10:G11"/>
-    <mergeCell ref="H10:I11"/>
-    <mergeCell ref="J10:K11"/>
-    <mergeCell ref="D12:E13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="H12:I13"/>
-    <mergeCell ref="J12:K13"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="F6:G7"/>
-    <mergeCell ref="H6:I7"/>
-    <mergeCell ref="J6:K7"/>
-    <mergeCell ref="J8:K9"/>
-    <mergeCell ref="H8:I9"/>
-    <mergeCell ref="F8:G9"/>
-    <mergeCell ref="D8:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>